<commit_message>
added MCU and Power conn
</commit_message>
<xml_diff>
--- a/BOM/BOM temp.xlsx
+++ b/BOM/BOM temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\github_folders\Dsp-guitar-effect\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712157AC-EB16-4F17-9908-9DA4F63BA363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C57AE6-BCD4-45AB-B4F9-835D7F6F19FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -101,15 +101,42 @@
   </si>
   <si>
     <t>https://www.reichelt.com/index.html?ACTION=7&amp;LA=3&amp;OPEN=0&amp;INDEX=0&amp;FILENAME=C700%2F1590BB.pdf</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>STM32H742VGT6</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>https://www.st.com/resource/en/datasheet/stm32h743zg.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.nl/nl/products/detail/stmicroelectronics/STM32H742VGT6/12337748</t>
+  </si>
+  <si>
+    <t>POWER INPUT JACK</t>
+  </si>
+  <si>
+    <t>WURTH</t>
+  </si>
+  <si>
+    <t>694106301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/katalog/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.be/en/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,10 +175,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,18 +473,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FB3928-3411-4D37-BA6A-18EB1E3A66CA}">
-  <dimension ref="B3:H7"/>
+  <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="2" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
@@ -471,7 +498,7 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
@@ -494,13 +521,13 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>13.3584</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -514,13 +541,13 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.75</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -534,7 +561,7 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.22</v>
       </c>
       <c r="H6" t="s">
@@ -551,14 +578,54 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>10.88</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2">
+        <v>15.8147</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.1374</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -567,8 +634,10 @@
     <hyperlink ref="G4" r:id="rId2" xr:uid="{53CD514D-4AEE-4F9F-A34C-97E63F0C1344}"/>
     <hyperlink ref="H5" r:id="rId3" xr:uid="{9E71588C-5886-4511-B279-1A8CE62FE8EE}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{C36C13DD-3115-450F-8209-F7FF787697E8}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{070F9B93-9312-4953-849D-A776CA8031BF}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{03DF052A-07EC-4848-BBA6-89F4BF0E2316}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>